<commit_message>
Learning con dati scalati e usando ravel() (sbagliato a far commit)
</commit_message>
<xml_diff>
--- a/Studi & Appunti/Datasets/Prove Datasets.xlsx
+++ b/Studi & Appunti/Datasets/Prove Datasets.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
   <si>
     <t>Nome Dataset</t>
   </si>
@@ -37,6 +37,9 @@
     <t>Leap Usato Per Dataset (Leap1 = Quello che usa Daniele ; Leap2 = Quello che usa Antonino)</t>
   </si>
   <si>
+    <t>NOTE</t>
+  </si>
+  <si>
     <t>Dataset Daniele</t>
   </si>
   <si>
@@ -89,13 +92,28 @@
   </si>
   <si>
     <t>7-10min</t>
+  </si>
+  <si>
+    <t>Dataset 20 righe v.3</t>
+  </si>
+  <si>
+    <t>5 min</t>
+  </si>
+  <si>
+    <t>Gianluca(5 jobs)</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Usato ravel() per risolvere DataConversionWarning. usato i valori scalati, quindi ricordarsi si usare la funz per scalare le features quando si testa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -103,10 +121,18 @@
     </font>
     <font>
       <b/>
+      <sz val="11.0"/>
       <color rgb="FFCC0000"/>
-      <name val="Montserrat"/>
+      <name val="EB Garamond"/>
     </font>
-    <font/>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="EB Garamond"/>
+    </font>
     <font>
       <name val="Montserrat"/>
     </font>
@@ -141,7 +167,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -160,17 +186,21 @@
     <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -389,21 +419,22 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="20.57"/>
     <col customWidth="1" min="2" max="2" width="22.57"/>
-    <col customWidth="1" min="3" max="3" width="27.14"/>
+    <col customWidth="1" min="3" max="3" width="15.71"/>
     <col customWidth="1" min="4" max="4" width="18.43"/>
     <col customWidth="1" min="5" max="5" width="20.71"/>
     <col customWidth="1" min="7" max="7" width="24.29"/>
-    <col customWidth="1" min="8" max="8" width="43.43"/>
+    <col customWidth="1" min="8" max="8" width="31.86"/>
+    <col customWidth="1" min="9" max="9" width="50.0"/>
   </cols>
   <sheetData>
-    <row r="1" ht="36.75" customHeight="1">
+    <row r="1" ht="47.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -421,352 +452,373 @@
       <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4"/>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="5">
         <v>500.0</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="5">
         <v>0.9975</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="6" t="s">
         <v>13</v>
       </c>
+      <c r="H2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="6"/>
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="5">
         <v>500.0</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F3" s="5">
         <v>1.0</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="7"/>
+        <v>16</v>
+      </c>
+      <c r="I3" s="6"/>
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="5">
         <v>500.0</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F4" s="5">
         <v>1.0</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" s="7"/>
+        <v>19</v>
+      </c>
+      <c r="I4" s="6"/>
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" s="5">
         <v>20.0</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F5" s="5">
         <v>0.7</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="7"/>
+        <v>24</v>
+      </c>
+      <c r="I5" s="6"/>
     </row>
     <row r="6">
       <c r="A6" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" s="5">
         <v>20.0</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F6" s="5">
         <v>0.97</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" s="7"/>
+        <v>24</v>
+      </c>
+      <c r="I6" s="6"/>
     </row>
     <row r="7">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="7"/>
+      <c r="A7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="5">
+        <v>20.0</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="7"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
     </row>
     <row r="9">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
       <c r="I9" s="7"/>
     </row>
     <row r="10">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
       <c r="I10" s="7"/>
     </row>
     <row r="11">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
       <c r="I11" s="7"/>
     </row>
     <row r="12">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
       <c r="H12" s="8"/>
       <c r="I12" s="7"/>
     </row>
     <row r="13">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
       <c r="I13" s="7"/>
     </row>
     <row r="14">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
       <c r="I14" s="7"/>
     </row>
     <row r="15">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
       <c r="I15" s="7"/>
     </row>
     <row r="16">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
       <c r="I16" s="7"/>
     </row>
     <row r="17">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
       <c r="I17" s="7"/>
     </row>
     <row r="18">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
       <c r="I18" s="7"/>
     </row>
     <row r="19">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
       <c r="I19" s="7"/>
     </row>
     <row r="20">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
       <c r="I20" s="7"/>
     </row>
     <row r="21">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
       <c r="I21" s="7"/>
     </row>
     <row r="22">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
       <c r="I22" s="7"/>
     </row>
     <row r="23">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
       <c r="I23" s="7"/>
     </row>
     <row r="24">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
       <c r="I24" s="7"/>
     </row>
     <row r="25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
       <c r="I25" s="7"/>
     </row>
     <row r="26">
@@ -777,7 +829,7 @@
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
+      <c r="H26" s="7"/>
       <c r="I26" s="7"/>
     </row>
     <row r="27">
@@ -788,7 +840,7 @@
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
+      <c r="H27" s="7"/>
       <c r="I27" s="7"/>
     </row>
     <row r="28">
@@ -799,7 +851,7 @@
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
+      <c r="H28" s="7"/>
       <c r="I28" s="7"/>
     </row>
     <row r="29">
@@ -810,96 +862,102 @@
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
+      <c r="H29" s="7"/>
       <c r="I29" s="7"/>
     </row>
     <row r="30">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="11"/>
     </row>
     <row r="31">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="11"/>
     </row>
     <row r="32">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="11"/>
     </row>
     <row r="33">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
+      <c r="A33" s="11"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="11"/>
     </row>
     <row r="34">
-      <c r="A34" s="7"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="7"/>
+      <c r="A34" s="11"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="11"/>
     </row>
     <row r="35">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
-      <c r="I35" s="7"/>
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="11"/>
     </row>
     <row r="36">
-      <c r="A36" s="7"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
-      <c r="I36" s="7"/>
+      <c r="A36" s="11"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="11"/>
     </row>
     <row r="37">
-      <c r="A37" s="7"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="7"/>
-      <c r="I37" s="7"/>
+      <c r="A37" s="11"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="11"/>
+    </row>
+    <row r="38">
+      <c r="H38" s="11"/>
+    </row>
+    <row r="39">
+      <c r="H39" s="11"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
tasto learning funziona. prende dataset da appdata e scrive risultati li. Lo script .py viene generato dall'applicazione, partendo dal file .txt in Resources/Text. Nuovi calcoli.
</commit_message>
<xml_diff>
--- a/Studi & Appunti/Datasets/Prove Datasets.xlsx
+++ b/Studi & Appunti/Datasets/Prove Datasets.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="36">
   <si>
     <t>Nome Dataset</t>
   </si>
@@ -49,7 +49,7 @@
     <t>140 min</t>
   </si>
   <si>
-    <t>Daniele</t>
+    <t>Daniele(20 jobs)</t>
   </si>
   <si>
     <t>N</t>
@@ -107,6 +107,18 @@
   </si>
   <si>
     <t>Usato ravel() per risolvere DataConversionWarning. usato i valori scalati, quindi ricordarsi si usare la funz per scalare le features quando si testa</t>
+  </si>
+  <si>
+    <t>Dataset 20 righe v.4</t>
+  </si>
+  <si>
+    <t>10 min</t>
+  </si>
+  <si>
+    <t>Dataset 20 righe v.5</t>
+  </si>
+  <si>
+    <t>14 min</t>
   </si>
 </sst>
 </file>
@@ -167,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -186,13 +198,7 @@
     <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
     <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -484,7 +490,7 @@
       <c r="H2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="6"/>
+      <c r="I2" s="5"/>
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
@@ -511,7 +517,7 @@
       <c r="H3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="6"/>
+      <c r="I3" s="5"/>
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
@@ -538,7 +544,7 @@
       <c r="H4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="6"/>
+      <c r="I4" s="5"/>
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
@@ -565,7 +571,7 @@
       <c r="H5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="6"/>
+      <c r="I5" s="5"/>
     </row>
     <row r="6">
       <c r="A6" s="5" t="s">
@@ -592,7 +598,7 @@
       <c r="H6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="6"/>
+      <c r="I6" s="5"/>
     </row>
     <row r="7">
       <c r="A7" s="5" t="s">
@@ -624,340 +630,374 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
+      <c r="A8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="5">
+        <v>20.0</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
+      <c r="A9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="5">
+        <v>20.0</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="5"/>
     </row>
     <row r="10">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
     </row>
     <row r="11">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
     </row>
     <row r="12">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="7"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
     </row>
     <row r="13">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
     </row>
     <row r="14">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
     </row>
     <row r="15">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
     </row>
     <row r="16">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
     </row>
     <row r="17">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
     </row>
     <row r="18">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
     </row>
     <row r="19">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
     </row>
     <row r="20">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
     </row>
     <row r="21">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
     </row>
     <row r="22">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
     </row>
     <row r="23">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
     </row>
     <row r="24">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
     </row>
     <row r="25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
     </row>
     <row r="26">
-      <c r="A26" s="9"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
     </row>
     <row r="27">
-      <c r="A27" s="9"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
     </row>
     <row r="28">
-      <c r="A28" s="10"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
     </row>
     <row r="29">
-      <c r="A29" s="10"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
+      <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
     </row>
     <row r="30">
-      <c r="A30" s="11"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="11"/>
+      <c r="A30" s="9"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="9"/>
     </row>
     <row r="31">
-      <c r="A31" s="11"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="11"/>
+      <c r="A31" s="9"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="9"/>
     </row>
     <row r="32">
-      <c r="A32" s="11"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="12"/>
-      <c r="I32" s="11"/>
+      <c r="A32" s="9"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="9"/>
     </row>
     <row r="33">
-      <c r="A33" s="11"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="11"/>
+      <c r="A33" s="9"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="9"/>
     </row>
     <row r="34">
-      <c r="A34" s="11"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="11"/>
+      <c r="A34" s="9"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="9"/>
     </row>
     <row r="35">
-      <c r="A35" s="11"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="12"/>
-      <c r="I35" s="11"/>
+      <c r="A35" s="9"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="9"/>
     </row>
     <row r="36">
-      <c r="A36" s="11"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="12"/>
-      <c r="I36" s="11"/>
+      <c r="A36" s="9"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="9"/>
     </row>
     <row r="37">
-      <c r="A37" s="11"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="12"/>
-      <c r="I37" s="11"/>
+      <c r="A37" s="9"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="9"/>
     </row>
     <row r="38">
-      <c r="H38" s="11"/>
+      <c r="H38" s="9"/>
     </row>
     <row r="39">
-      <c r="H39" s="11"/>
+      <c r="H39" s="9"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
aggiunto documentazione, aggiunto commenti, eseguito nuovo calcolo su dataset misto ma scalando i dati, aggiunto valori sul file excel
</commit_message>
<xml_diff>
--- a/Studi & Appunti/Datasets/Prove Datasets.xlsx
+++ b/Studi & Appunti/Datasets/Prove Datasets.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DEV\C# UNITY\Projects\MarcoSmiles\Studi &amp; Appunti\Datasets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE01284-28BC-442B-9F5C-A8BED6107928}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Foglio1" sheetId="1" r:id="rId4"/>
+    <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
   <si>
     <t>Nome Dataset</t>
   </si>
@@ -124,33 +133,41 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FFCC0000"/>
       <name val="EB Garamond"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <name val="EB Garamond"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Montserrat"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Montserrat"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="EB Garamond"/>
     </font>
   </fonts>
   <fills count="4">
@@ -158,7 +175,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -174,53 +191,65 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="12">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -410,30 +439,35 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.57"/>
-    <col customWidth="1" min="2" max="2" width="22.57"/>
-    <col customWidth="1" min="3" max="3" width="15.71"/>
-    <col customWidth="1" min="4" max="4" width="18.43"/>
-    <col customWidth="1" min="5" max="5" width="20.71"/>
-    <col customWidth="1" min="7" max="7" width="24.29"/>
-    <col customWidth="1" min="8" max="8" width="31.86"/>
-    <col customWidth="1" min="9" max="9" width="50.0"/>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="24.28515625" customWidth="1"/>
+    <col min="8" max="8" width="31.85546875" customWidth="1"/>
+    <col min="9" max="9" width="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="47.25" customHeight="1">
+    <row r="1" spans="1:12" ht="47.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -465,7 +499,7 @@
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:12" ht="14.25">
       <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
@@ -473,7 +507,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="5">
-        <v>500.0</v>
+        <v>500</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>11</v>
@@ -482,7 +516,7 @@
         <v>12</v>
       </c>
       <c r="F2" s="5">
-        <v>0.9975</v>
+        <v>0.99750000000000005</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>13</v>
@@ -492,7 +526,7 @@
       </c>
       <c r="I2" s="5"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:12" ht="14.25">
       <c r="A3" s="5" t="s">
         <v>15</v>
       </c>
@@ -500,7 +534,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="5">
-        <v>500.0</v>
+        <v>500</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>11</v>
@@ -509,7 +543,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>13</v>
@@ -519,7 +553,7 @@
       </c>
       <c r="I3" s="5"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:12" ht="28.5">
       <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
@@ -527,7 +561,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="5">
-        <v>500.0</v>
+        <v>500</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>18</v>
@@ -536,7 +570,7 @@
         <v>12</v>
       </c>
       <c r="F4" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>13</v>
@@ -546,7 +580,7 @@
       </c>
       <c r="I4" s="5"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:12" ht="28.5">
       <c r="A5" s="5" t="s">
         <v>20</v>
       </c>
@@ -554,7 +588,7 @@
         <v>21</v>
       </c>
       <c r="C5" s="5">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>22</v>
@@ -573,7 +607,7 @@
       </c>
       <c r="I5" s="5"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:12" ht="14.25">
       <c r="A6" s="5" t="s">
         <v>25</v>
       </c>
@@ -581,7 +615,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="5">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>26</v>
@@ -600,7 +634,7 @@
       </c>
       <c r="I6" s="5"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:12" ht="57">
       <c r="A7" s="5" t="s">
         <v>27</v>
       </c>
@@ -608,7 +642,7 @@
         <v>21</v>
       </c>
       <c r="C7" s="5">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>28</v>
@@ -617,7 +651,7 @@
         <v>29</v>
       </c>
       <c r="F7" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>30</v>
@@ -629,7 +663,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:12" ht="57">
       <c r="A8" s="5" t="s">
         <v>32</v>
       </c>
@@ -637,7 +671,7 @@
         <v>10</v>
       </c>
       <c r="C8" s="5">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>33</v>
@@ -646,7 +680,7 @@
         <v>29</v>
       </c>
       <c r="F8" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>30</v>
@@ -654,11 +688,11 @@
       <c r="H8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:12" ht="14.25">
       <c r="A9" s="5" t="s">
         <v>34</v>
       </c>
@@ -666,7 +700,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="5">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>35</v>
@@ -675,7 +709,7 @@
         <v>29</v>
       </c>
       <c r="F9" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>13</v>
@@ -685,18 +719,34 @@
       </c>
       <c r="I9" s="5"/>
     </row>
-    <row r="10">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
+    <row r="10" spans="1:12" ht="28.5">
+      <c r="A10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="5">
+        <v>500</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0.99980000000000002</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="I10" s="5"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:12" ht="14.25">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -707,7 +757,7 @@
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:12" ht="14.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -718,7 +768,7 @@
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:12" ht="14.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -729,7 +779,7 @@
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:12" ht="12.75">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -740,7 +790,7 @@
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:12" ht="12.75">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -751,7 +801,7 @@
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:12" ht="12.75">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -762,7 +812,7 @@
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:9" ht="12.75">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -773,7 +823,7 @@
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:9" ht="12.75">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -784,7 +834,7 @@
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:9" ht="12.75">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -795,7 +845,7 @@
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:9" ht="12.75">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -806,7 +856,7 @@
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:9" ht="12.75">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -817,7 +867,7 @@
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:9" ht="12.75">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -828,7 +878,7 @@
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:9" ht="12.75">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -839,7 +889,7 @@
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:9" ht="12.75">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -850,7 +900,7 @@
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:9" ht="12.75">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -861,7 +911,7 @@
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:9" ht="12.75">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
@@ -872,7 +922,7 @@
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:9" ht="12.75">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
@@ -883,7 +933,7 @@
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:9" ht="12.75">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
@@ -894,7 +944,7 @@
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:9" ht="12.75">
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
@@ -905,7 +955,7 @@
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:9" ht="12.75">
       <c r="A30" s="9"/>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
@@ -916,7 +966,7 @@
       <c r="H30" s="10"/>
       <c r="I30" s="9"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:9" ht="12.75">
       <c r="A31" s="9"/>
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
@@ -927,7 +977,7 @@
       <c r="H31" s="10"/>
       <c r="I31" s="9"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:9" ht="12.75">
       <c r="A32" s="9"/>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
@@ -938,7 +988,7 @@
       <c r="H32" s="10"/>
       <c r="I32" s="9"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:9" ht="12.75">
       <c r="A33" s="9"/>
       <c r="B33" s="9"/>
       <c r="C33" s="9"/>
@@ -949,7 +999,7 @@
       <c r="H33" s="10"/>
       <c r="I33" s="9"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:9" ht="12.75">
       <c r="A34" s="9"/>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
@@ -960,7 +1010,7 @@
       <c r="H34" s="10"/>
       <c r="I34" s="9"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:9" ht="12.75">
       <c r="A35" s="9"/>
       <c r="B35" s="9"/>
       <c r="C35" s="9"/>
@@ -971,7 +1021,7 @@
       <c r="H35" s="10"/>
       <c r="I35" s="9"/>
     </row>
-    <row r="36">
+    <row r="36" spans="1:9" ht="12.75">
       <c r="A36" s="9"/>
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
@@ -982,7 +1032,7 @@
       <c r="H36" s="10"/>
       <c r="I36" s="9"/>
     </row>
-    <row r="37">
+    <row r="37" spans="1:9" ht="12.75">
       <c r="A37" s="9"/>
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
@@ -993,13 +1043,14 @@
       <c r="H37" s="10"/>
       <c r="I37" s="9"/>
     </row>
-    <row r="38">
+    <row r="38" spans="1:9" ht="12.75">
       <c r="H38" s="9"/>
     </row>
-    <row r="39">
+    <row r="39" spans="1:9" ht="12.75">
       <c r="H39" s="9"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
sistemato caricamento note già registrate, aggiunto dataset alla cartella dei dataset
</commit_message>
<xml_diff>
--- a/Studi & Appunti/Datasets/Prove Datasets.xlsx
+++ b/Studi & Appunti/Datasets/Prove Datasets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DEV\C# UNITY\Projects\MarcoSmiles\Studi &amp; Appunti\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE01284-28BC-442B-9F5C-A8BED6107928}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4DE1A89-5227-4C66-8806-C19E45541357}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="38">
   <si>
     <t>Nome Dataset</t>
   </si>
@@ -128,6 +128,12 @@
   </si>
   <si>
     <t>14 min</t>
+  </si>
+  <si>
+    <t>Dataset Daniele 1 ottava</t>
+  </si>
+  <si>
+    <t>20 min</t>
   </si>
 </sst>
 </file>
@@ -452,7 +458,7 @@
   <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -746,15 +752,31 @@
       </c>
       <c r="I10" s="5"/>
     </row>
-    <row r="11" spans="1:12" ht="14.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
+    <row r="11" spans="1:12" ht="28.5">
+      <c r="A11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="5">
+        <v>500</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="5">
+        <v>1</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:12" ht="14.25">

</xml_diff>